<commit_message>
- implemented `nexial.scope.refetchDataFile` to preserve data variable changes between iteration.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/plan/disable-showcase-plan.xlsx
+++ b/src/test/resources/showcase/artifact/plan/disable-showcase-plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C39BF94-C00C-754E-B559-CDB87510889B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4D3422-DEED-A148-B853-876F08A39FBC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="16220" windowWidth="25600" windowHeight="15780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="25160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="2" r:id="rId1"/>
@@ -852,7 +852,7 @@
   <dimension ref="A1:N700"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>